<commit_message>
dc read spi regs
</commit_message>
<xml_diff>
--- a/documents/Addressing.xlsx
+++ b/documents/Addressing.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\100.90.211.128\eyhc\acme\NANO_QLASER\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\Eric\acme\NANO_QLASER\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8911D91F-A791-418D-AF34-1519C59457A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E05147-5E8A-4A87-8868-E40600D4CF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Addressing" sheetId="2" r:id="rId1"/>
     <sheet name="Pulse Channel" sheetId="1" r:id="rId2"/>
     <sheet name="ACChannels Registers" sheetId="3" r:id="rId3"/>
     <sheet name="Misc Registers" sheetId="4" r:id="rId4"/>
+    <sheet name="DC Address" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>bits
 Addr</t>
@@ -125,6 +126,53 @@
   <si>
     <t>bits
 Register</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bits
+Read/Write
+</t>
+  </si>
+  <si>
+    <t>Channel (If command is SPIn)</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Command Value</t>
+  </si>
+  <si>
+    <t>SPI0</t>
+  </si>
+  <si>
+    <t>SPI1</t>
+  </si>
+  <si>
+    <t>SPI2</t>
+  </si>
+  <si>
+    <t>SPI3</t>
+  </si>
+  <si>
+    <t>SPI All</t>
+  </si>
+  <si>
+    <t>Internal Reference</t>
+  </si>
+  <si>
+    <t>DAC Power On</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Read Command</t>
   </si>
 </sst>
 </file>
@@ -328,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="135" wrapText="1"/>
@@ -337,80 +385,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,17 +408,81 @@
       <alignment horizontal="center" vertical="center" textRotation="135" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,41 +769,41 @@
       <selection activeCell="R2" sqref="R2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" customWidth="1"/>
-    <col min="2" max="2" width="3.54296875" customWidth="1"/>
-    <col min="3" max="3" width="3.81640625" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" customWidth="1"/>
-    <col min="7" max="7" width="3.81640625" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.54296875" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" customWidth="1"/>
-    <col min="12" max="12" width="3.7265625" customWidth="1"/>
-    <col min="13" max="13" width="3.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="3.453125" customWidth="1"/>
-    <col min="16" max="16" width="3.26953125" customWidth="1"/>
-    <col min="17" max="17" width="3.81640625" customWidth="1"/>
-    <col min="18" max="18" width="3.453125" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
     <col min="19" max="20" width="4" customWidth="1"/>
-    <col min="21" max="21" width="5.08984375" customWidth="1"/>
-    <col min="22" max="22" width="3.7265625" customWidth="1"/>
-    <col min="23" max="23" width="3.81640625" customWidth="1"/>
-    <col min="24" max="24" width="3.26953125" customWidth="1"/>
-    <col min="25" max="25" width="3.54296875" customWidth="1"/>
-    <col min="26" max="26" width="3.81640625" customWidth="1"/>
-    <col min="27" max="27" width="3.453125" customWidth="1"/>
-    <col min="28" max="30" width="3.1796875" customWidth="1"/>
-    <col min="31" max="31" width="3.26953125" customWidth="1"/>
-    <col min="32" max="32" width="3.453125" customWidth="1"/>
-    <col min="33" max="33" width="4.81640625" customWidth="1"/>
+    <col min="21" max="21" width="5.140625" customWidth="1"/>
+    <col min="22" max="22" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" customWidth="1"/>
+    <col min="25" max="25" width="3.5703125" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+    <col min="28" max="30" width="3.140625" customWidth="1"/>
+    <col min="31" max="31" width="3.28515625" customWidth="1"/>
+    <col min="32" max="32" width="3.42578125" customWidth="1"/>
+    <col min="33" max="33" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -852,53 +904,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="19" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:33" s="6" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="20" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="21" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="25" t="s">
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="25"/>
-    </row>
-    <row r="3" spans="1:33" s="19" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:33" ht="58.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="AG2" s="16"/>
+    </row>
+    <row r="3" spans="1:33" s="6" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:33" ht="58.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="AF2:AG2"/>
@@ -915,44 +967,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" customWidth="1"/>
-    <col min="2" max="2" width="3.54296875" customWidth="1"/>
-    <col min="3" max="3" width="3.81640625" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" customWidth="1"/>
-    <col min="7" max="7" width="3.81640625" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.54296875" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" customWidth="1"/>
-    <col min="12" max="12" width="3.7265625" customWidth="1"/>
-    <col min="13" max="13" width="3.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="3.453125" customWidth="1"/>
-    <col min="16" max="16" width="3.26953125" customWidth="1"/>
-    <col min="17" max="17" width="3.81640625" customWidth="1"/>
-    <col min="18" max="18" width="3.453125" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
     <col min="19" max="20" width="4" customWidth="1"/>
-    <col min="21" max="22" width="3.7265625" customWidth="1"/>
-    <col min="23" max="23" width="3.81640625" customWidth="1"/>
-    <col min="24" max="24" width="3.26953125" customWidth="1"/>
-    <col min="25" max="25" width="3.54296875" customWidth="1"/>
-    <col min="26" max="26" width="3.81640625" customWidth="1"/>
-    <col min="27" max="27" width="3.453125" customWidth="1"/>
-    <col min="28" max="30" width="3.1796875" customWidth="1"/>
-    <col min="31" max="31" width="3.26953125" customWidth="1"/>
-    <col min="32" max="32" width="3.453125" customWidth="1"/>
-    <col min="33" max="33" width="3.1796875" customWidth="1"/>
+    <col min="21" max="22" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" customWidth="1"/>
+    <col min="25" max="25" width="3.5703125" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+    <col min="28" max="30" width="3.140625" customWidth="1"/>
+    <col min="31" max="31" width="3.28515625" customWidth="1"/>
+    <col min="32" max="32" width="3.42578125" customWidth="1"/>
+    <col min="33" max="33" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,142 +1105,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="8"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="26"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="11"/>
-      <c r="V3" s="9" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="27"/>
+      <c r="V3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="11"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="27"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="12" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="14"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="23"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="14"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="23"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
   </sheetData>
@@ -1209,47 +1261,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D398F2B2-371A-41B8-9328-D15B6F64B98C}">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AT19" sqref="AT19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="3.54296875" customWidth="1"/>
-    <col min="3" max="3" width="3.81640625" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" customWidth="1"/>
-    <col min="7" max="7" width="3.81640625" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.54296875" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" customWidth="1"/>
-    <col min="12" max="12" width="3.7265625" customWidth="1"/>
-    <col min="13" max="13" width="3.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="3.453125" customWidth="1"/>
-    <col min="16" max="16" width="3.26953125" customWidth="1"/>
-    <col min="17" max="17" width="3.81640625" customWidth="1"/>
-    <col min="18" max="18" width="3.453125" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
     <col min="19" max="20" width="4" customWidth="1"/>
-    <col min="21" max="22" width="3.7265625" customWidth="1"/>
-    <col min="23" max="23" width="3.81640625" customWidth="1"/>
-    <col min="24" max="24" width="3.26953125" customWidth="1"/>
-    <col min="25" max="25" width="3.54296875" customWidth="1"/>
-    <col min="26" max="26" width="3.81640625" customWidth="1"/>
-    <col min="27" max="27" width="3.453125" customWidth="1"/>
-    <col min="28" max="28" width="3.1796875" customWidth="1"/>
-    <col min="29" max="29" width="4.54296875" customWidth="1"/>
-    <col min="30" max="30" width="3.1796875" customWidth="1"/>
-    <col min="31" max="31" width="3.26953125" customWidth="1"/>
-    <col min="32" max="32" width="3.453125" customWidth="1"/>
-    <col min="33" max="33" width="8.90625" customWidth="1"/>
+    <col min="21" max="22" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" customWidth="1"/>
+    <col min="25" max="25" width="3.5703125" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+    <col min="28" max="28" width="3.140625" customWidth="1"/>
+    <col min="29" max="29" width="4.5703125" customWidth="1"/>
+    <col min="30" max="30" width="3.140625" customWidth="1"/>
+    <col min="31" max="31" width="3.28515625" customWidth="1"/>
+    <col min="32" max="32" width="3.42578125" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:35" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="4">
@@ -1348,253 +1400,253 @@
       <c r="AG1" s="4">
         <v>0</v>
       </c>
-      <c r="AI1" s="31" t="s">
+      <c r="AI1" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A2" s="22">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="30" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A3" s="22">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17"/>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A4" s="22">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-    </row>
-    <row r="5" spans="1:35" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="22">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+    </row>
+    <row r="5" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="29" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AD5" s="24">
+      <c r="AD5" s="33">
         <v>0</v>
       </c>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="32" t="s">
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A6" s="22">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="21"/>
-      <c r="AF6" s="21"/>
-      <c r="AG6" s="21"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A7" s="22">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="18"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="17" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="17"/>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="17"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1621,44 +1673,42 @@
       <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="3.54296875" customWidth="1"/>
-    <col min="3" max="3" width="3.81640625" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" customWidth="1"/>
-    <col min="7" max="7" width="3.81640625" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" customWidth="1"/>
-    <col min="9" max="9" width="3.453125" customWidth="1"/>
-    <col min="10" max="10" width="3.54296875" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" customWidth="1"/>
-    <col min="12" max="12" width="3.7265625" customWidth="1"/>
-    <col min="13" max="13" width="3.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="3.453125" customWidth="1"/>
-    <col min="16" max="16" width="3.26953125" customWidth="1"/>
-    <col min="17" max="17" width="3.81640625" customWidth="1"/>
-    <col min="18" max="18" width="3.453125" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
     <col min="19" max="20" width="4" customWidth="1"/>
-    <col min="21" max="22" width="3.7265625" customWidth="1"/>
-    <col min="23" max="23" width="3.81640625" customWidth="1"/>
-    <col min="24" max="24" width="3.26953125" customWidth="1"/>
-    <col min="25" max="25" width="3.54296875" customWidth="1"/>
-    <col min="26" max="26" width="3.81640625" customWidth="1"/>
-    <col min="27" max="27" width="3.453125" customWidth="1"/>
-    <col min="28" max="28" width="3.1796875" customWidth="1"/>
-    <col min="29" max="29" width="3.08984375" customWidth="1"/>
-    <col min="30" max="30" width="3.1796875" customWidth="1"/>
-    <col min="31" max="31" width="3.26953125" customWidth="1"/>
-    <col min="32" max="32" width="3.453125" customWidth="1"/>
-    <col min="33" max="33" width="7.36328125" style="36" customWidth="1"/>
-    <col min="34" max="34" width="4.36328125" customWidth="1"/>
+    <col min="21" max="22" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" customWidth="1"/>
+    <col min="25" max="25" width="3.5703125" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+    <col min="28" max="30" width="3.140625" customWidth="1"/>
+    <col min="31" max="31" width="3.28515625" customWidth="1"/>
+    <col min="32" max="32" width="3.42578125" customWidth="1"/>
+    <col min="33" max="33" width="7.42578125" style="15" customWidth="1"/>
+    <col min="34" max="34" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:35" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="4">
@@ -1754,254 +1804,254 @@
       <c r="AF1" s="4">
         <v>1</v>
       </c>
-      <c r="AG1" s="35">
+      <c r="AG1" s="14">
         <v>0</v>
       </c>
-      <c r="AI1" s="31" t="s">
+      <c r="AI1" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A2" s="27">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A3" s="27">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="16"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="17" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A4" s="27">
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="17" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A5" s="27">
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="17" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="36"/>
+      <c r="X5" s="36"/>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="36"/>
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="17"/>
-    </row>
-    <row r="6" spans="1:35" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27">
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+    </row>
+    <row r="6" spans="1:35" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="28" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="34"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
+      <c r="AF6" s="35"/>
+      <c r="AG6" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27">
+    <row r="7" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="37"/>
-      <c r="AG7" s="28" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34"/>
+      <c r="AE7" s="34"/>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2020,4 +2070,310 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB8ABF5-761E-4EA7-A0D6-F2023441961B}">
+  <dimension ref="A1:AJ8"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
+    <col min="19" max="20" width="4" customWidth="1"/>
+    <col min="21" max="22" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" customWidth="1"/>
+    <col min="25" max="25" width="3.5703125" customWidth="1"/>
+    <col min="26" max="26" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" customWidth="1"/>
+    <col min="28" max="30" width="3.140625" customWidth="1"/>
+    <col min="31" max="31" width="7.7109375" customWidth="1"/>
+    <col min="32" max="32" width="8.140625" customWidth="1"/>
+    <col min="33" max="33" width="10.5703125" style="15" customWidth="1"/>
+    <col min="34" max="34" width="4.42578125" customWidth="1"/>
+    <col min="35" max="35" width="15.85546875" customWidth="1"/>
+    <col min="36" max="36" width="34.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2">
+        <v>21</v>
+      </c>
+      <c r="M1" s="2">
+        <v>20</v>
+      </c>
+      <c r="N1" s="2">
+        <v>19</v>
+      </c>
+      <c r="O1" s="2">
+        <v>18</v>
+      </c>
+      <c r="P1" s="2">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2">
+        <v>15</v>
+      </c>
+      <c r="S1" s="2">
+        <v>14</v>
+      </c>
+      <c r="T1" s="2">
+        <v>13</v>
+      </c>
+      <c r="U1" s="2">
+        <v>12</v>
+      </c>
+      <c r="V1" s="2">
+        <v>11</v>
+      </c>
+      <c r="W1" s="2">
+        <v>10</v>
+      </c>
+      <c r="X1" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>4</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG1" s="14">
+        <v>0</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="30"/>
+      <c r="AE3" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="AG4"/>
+      <c r="AI4">
+        <v>2</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="AG5"/>
+      <c r="AI5">
+        <v>3</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="AG6"/>
+      <c r="AI6">
+        <v>4</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="AG7"/>
+      <c r="AI7">
+        <v>5</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="AG8"/>
+      <c r="AI8">
+        <v>6</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update documentation and refine VHDL
</commit_message>
<xml_diff>
--- a/documents/Addressing.xlsx
+++ b/documents/Addressing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\Eric\acme\NANO_QLASER\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5D0A9-0824-4871-8760-43DFC1BC0400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079047C3-9413-49BE-A55E-E613583086E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Addressing" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="AC Channels" sheetId="3" r:id="rId3"/>
     <sheet name="DC Channels" sheetId="6" r:id="rId4"/>
     <sheet name="Misc Registers" sheetId="4" r:id="rId5"/>
+    <sheet name="fw_packet" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="109">
   <si>
     <t>bits
 Addr</t>
@@ -348,6 +349,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>data (groups of 32-bit packet)</t>
+  </si>
+  <si>
+    <t>packet size</t>
+  </si>
+  <si>
+    <t>command</t>
   </si>
 </sst>
 </file>
@@ -656,44 +666,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -998,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDC3AE2-1610-42F8-9495-7B1DB616FE66}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1475,7 @@
   <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="X3" sqref="X3:AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,16 +1608,16 @@
       <c r="C2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="40">
-        <v>0</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
+      <c r="D2" s="38">
+        <v>0</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="28" t="s">
         <v>1</v>
       </c>
@@ -1645,46 +1655,46 @@
       <c r="C3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="35">
-        <v>0</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
+      <c r="D3" s="37">
+        <v>0</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="28" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="29"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="36"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="41"/>
       <c r="T3" s="28">
         <v>0</v>
       </c>
       <c r="U3" s="29"/>
       <c r="V3" s="29"/>
       <c r="W3" s="30"/>
-      <c r="X3" s="39" t="s">
+      <c r="X3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="36"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="41"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1743,26 +1753,26 @@
       <c r="C5" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="33">
-        <v>0</v>
-      </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="39" t="s">
+      <c r="D5" s="34">
+        <v>0</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="35"/>
+      <c r="S5" s="37"/>
       <c r="T5" s="29"/>
       <c r="U5" s="29"/>
       <c r="V5" s="29"/>
@@ -1781,43 +1791,43 @@
       <c r="AI5" s="30"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="42"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
-      <c r="AD6" s="42"/>
-      <c r="AE6" s="42"/>
-      <c r="AF6" s="42"/>
-      <c r="AG6" s="42"/>
-      <c r="AH6" s="42"/>
-      <c r="AI6" s="43"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="40"/>
       <c r="AK6" s="9"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -1830,26 +1840,26 @@
       <c r="C7" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="38" t="s">
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="38"/>
+      <c r="S7" s="33"/>
       <c r="T7" s="22"/>
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
@@ -1916,43 +1926,43 @@
       <c r="AK8" s="9"/>
     </row>
     <row r="9" spans="1:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
-      <c r="Y9" s="40"/>
-      <c r="Z9" s="40"/>
-      <c r="AA9" s="40"/>
-      <c r="AB9" s="40"/>
-      <c r="AC9" s="40"/>
-      <c r="AD9" s="40"/>
-      <c r="AE9" s="40"/>
-      <c r="AF9" s="40"/>
-      <c r="AG9" s="40"/>
-      <c r="AH9" s="40"/>
-      <c r="AI9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -2012,42 +2022,42 @@
       <c r="C11" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="35">
-        <v>0</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="37" t="s">
+      <c r="D11" s="37">
+        <v>0</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="38"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
+      <c r="AF11" s="33"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="33"/>
+      <c r="AI11" s="33"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -2181,11 +2191,11 @@
       <c r="AE14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AF14" s="33">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="33"/>
-      <c r="AH14" s="33"/>
+      <c r="AF14" s="34">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="34"/>
+      <c r="AH14" s="34"/>
       <c r="AI14" s="15" t="s">
         <v>13</v>
       </c>
@@ -2245,16 +2255,16 @@
       <c r="C16" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="33">
-        <v>0</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="34"/>
+      <c r="D16" s="34">
+        <v>0</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
       <c r="L16" s="22" t="s">
         <v>101</v>
       </c>
@@ -2509,6 +2519,28 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="D15:AI15"/>
+    <mergeCell ref="L16:AI16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D14:AD14"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="L11:AI11"/>
+    <mergeCell ref="D12:AI12"/>
+    <mergeCell ref="D13:AI13"/>
+    <mergeCell ref="AF14:AH14"/>
+    <mergeCell ref="D17:AI17"/>
+    <mergeCell ref="D18:AI18"/>
+    <mergeCell ref="D19:AI19"/>
+    <mergeCell ref="D20:AI20"/>
+    <mergeCell ref="D21:AI21"/>
+    <mergeCell ref="L2:AI2"/>
+    <mergeCell ref="J3:S3"/>
+    <mergeCell ref="X3:AI3"/>
+    <mergeCell ref="D4:S4"/>
+    <mergeCell ref="T4:AI4"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="D3:I3"/>
     <mergeCell ref="D10:S10"/>
     <mergeCell ref="T10:AI10"/>
     <mergeCell ref="R7:AI7"/>
@@ -2519,28 +2551,6 @@
     <mergeCell ref="D8:S8"/>
     <mergeCell ref="A6:AI6"/>
     <mergeCell ref="A9:AI9"/>
-    <mergeCell ref="L2:AI2"/>
-    <mergeCell ref="J3:S3"/>
-    <mergeCell ref="X3:AI3"/>
-    <mergeCell ref="D4:S4"/>
-    <mergeCell ref="T4:AI4"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="D17:AI17"/>
-    <mergeCell ref="D18:AI18"/>
-    <mergeCell ref="D19:AI19"/>
-    <mergeCell ref="D20:AI20"/>
-    <mergeCell ref="D21:AI21"/>
-    <mergeCell ref="D15:AI15"/>
-    <mergeCell ref="L16:AI16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="D14:AD14"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="L11:AI11"/>
-    <mergeCell ref="D12:AI12"/>
-    <mergeCell ref="D13:AI13"/>
-    <mergeCell ref="AF14:AH14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2683,12 +2693,12 @@
       <c r="C2" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="45">
-        <v>0</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="D2" s="44">
+        <v>0</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="7">
         <v>0</v>
       </c>
@@ -2726,52 +2736,52 @@
       <c r="AB2" s="47">
         <v>0</v>
       </c>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
     </row>
     <row r="3" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="44"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -2783,12 +2793,12 @@
       <c r="C4" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="45">
-        <v>0</v>
-      </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="D4" s="44">
+        <v>0</v>
+      </c>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="7">
         <v>0</v>
       </c>
@@ -2826,13 +2836,13 @@
       <c r="AB4" s="47">
         <v>0</v>
       </c>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="45"/>
-      <c r="AF4" s="45"/>
-      <c r="AG4" s="45"/>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="45"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="44"/>
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="44"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -2844,12 +2854,12 @@
       <c r="C5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="45">
-        <v>0</v>
-      </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="D5" s="44">
+        <v>0</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="7">
         <v>0</v>
       </c>
@@ -2899,12 +2909,12 @@
       <c r="C6" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="42">
-        <v>0</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="D6" s="39">
+        <v>0</v>
+      </c>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="7">
         <v>1</v>
       </c>
@@ -2917,24 +2927,24 @@
       <c r="K6" s="7">
         <v>0</v>
       </c>
-      <c r="L6" s="44">
-        <v>0</v>
-      </c>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="43"/>
+      <c r="L6" s="45">
+        <v>0</v>
+      </c>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="40"/>
       <c r="AB6" s="7">
         <v>0</v>
       </c>
@@ -2970,12 +2980,12 @@
       <c r="C7" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="D7" s="39">
+        <v>0</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="7">
         <v>0</v>
       </c>
@@ -3000,20 +3010,20 @@
       <c r="O7" s="7">
         <v>1</v>
       </c>
-      <c r="P7" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="43"/>
+      <c r="P7" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="39"/>
+      <c r="Z7" s="39"/>
+      <c r="AA7" s="40"/>
       <c r="AB7" s="7">
         <v>1</v>
       </c>
@@ -3049,36 +3059,36 @@
       <c r="C8" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="42">
-        <v>0</v>
-      </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="43"/>
+      <c r="D8" s="39">
+        <v>0</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="39"/>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="40"/>
       <c r="AF8" s="7" t="s">
         <v>85</v>
       </c>
@@ -3438,39 +3448,39 @@
       <c r="C6" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="40">
-        <v>0</v>
-      </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="40"/>
-      <c r="Z6" s="40"/>
-      <c r="AA6" s="40"/>
-      <c r="AB6" s="40"/>
-      <c r="AC6" s="40"/>
-      <c r="AD6" s="40"/>
-      <c r="AE6" s="40"/>
-      <c r="AF6" s="40"/>
-      <c r="AG6" s="40"/>
-      <c r="AH6" s="41"/>
+      <c r="D6" s="38">
+        <v>0</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="42"/>
       <c r="AI6" s="7" t="s">
         <v>20</v>
       </c>
@@ -3485,39 +3495,39 @@
       <c r="C7" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="40"/>
-      <c r="Z7" s="40"/>
-      <c r="AA7" s="40"/>
-      <c r="AB7" s="40"/>
-      <c r="AC7" s="40"/>
-      <c r="AD7" s="40"/>
-      <c r="AE7" s="40"/>
-      <c r="AF7" s="40"/>
-      <c r="AG7" s="40"/>
-      <c r="AH7" s="41"/>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="38"/>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="38"/>
+      <c r="AF7" s="38"/>
+      <c r="AG7" s="38"/>
+      <c r="AH7" s="42"/>
       <c r="AI7" s="7" t="s">
         <v>21</v>
       </c>
@@ -3537,4 +3547,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AAA558-C77A-4C0A-A112-4CDA524D2DDC}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
restructure firmware, and disable external ttl trigger for now
</commit_message>
<xml_diff>
--- a/documents/Addressing.xlsx
+++ b/documents/Addressing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\Eric\acme\NANO_QLASER\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5D0A9-0824-4871-8760-43DFC1BC0400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373F908A-198E-4DFE-AFE9-CBC4EEBD9092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Addressing" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Misc Registers" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="114">
   <si>
     <t>bits
 Addr</t>
@@ -290,21 +291,6 @@
     <t>SPI3 busy</t>
   </si>
   <si>
-    <t>Channel 0 select</t>
-  </si>
-  <si>
-    <t>Channel 0 Data</t>
-  </si>
-  <si>
-    <t>Channel 31 select</t>
-  </si>
-  <si>
-    <t>Channel 31 Data</t>
-  </si>
-  <si>
-    <t>0x001F</t>
-  </si>
-  <si>
     <t>0x0020</t>
   </si>
   <si>
@@ -348,6 +334,45 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>0x1011</t>
+  </si>
+  <si>
+    <t>Start time too early</t>
+  </si>
+  <si>
+    <t>Channel 0-7 select</t>
+  </si>
+  <si>
+    <t>Channel 0-7 Data</t>
+  </si>
+  <si>
+    <t>0x0008</t>
+  </si>
+  <si>
+    <t>Channel 8-15 select</t>
+  </si>
+  <si>
+    <t>Channel 8-15 Data</t>
+  </si>
+  <si>
+    <t>0x0010</t>
+  </si>
+  <si>
+    <t>Channel 16-23 select</t>
+  </si>
+  <si>
+    <t>Channel 16-23 Data</t>
+  </si>
+  <si>
+    <t>0x0018</t>
+  </si>
+  <si>
+    <t>Channel 24-31 select</t>
+  </si>
+  <si>
+    <t>Channel 24-31 Data</t>
   </si>
 </sst>
 </file>
@@ -656,44 +681,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -998,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDC3AE2-1610-42F8-9495-7B1DB616FE66}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
@@ -1462,7 +1487,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D398F2B2-371A-41B8-9328-D15B6F64B98C}">
-  <dimension ref="A1:AK21"/>
+  <dimension ref="A1:AK22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -1485,10 +1510,10 @@
         <v>76</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>44</v>
@@ -1596,18 +1621,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="40">
-        <v>0</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
+        <v>92</v>
+      </c>
+      <c r="D2" s="38">
+        <v>0</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="28" t="s">
         <v>1</v>
       </c>
@@ -1643,48 +1668,48 @@
         <v>0</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="35">
-        <v>0</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
+        <v>92</v>
+      </c>
+      <c r="D3" s="37">
+        <v>0</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="28" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="29"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="36"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="41"/>
       <c r="T3" s="28">
         <v>0</v>
       </c>
       <c r="U3" s="29"/>
       <c r="V3" s="29"/>
       <c r="W3" s="30"/>
-      <c r="X3" s="39" t="s">
+      <c r="X3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="36"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="41"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1694,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>5</v>
@@ -1741,28 +1766,28 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="33">
-        <v>0</v>
-      </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="34">
+        <v>0</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="35"/>
+      <c r="S5" s="37"/>
       <c r="T5" s="29"/>
       <c r="U5" s="29"/>
       <c r="V5" s="29"/>
@@ -1781,43 +1806,43 @@
       <c r="AI5" s="30"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="42"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
-      <c r="AD6" s="42"/>
-      <c r="AE6" s="42"/>
-      <c r="AF6" s="42"/>
-      <c r="AG6" s="42"/>
-      <c r="AH6" s="42"/>
-      <c r="AI6" s="43"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="40"/>
       <c r="AK6" s="9"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -1828,28 +1853,28 @@
         <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="38"/>
+      <c r="S7" s="33"/>
       <c r="T7" s="22"/>
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
@@ -1875,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>77</v>
@@ -1916,53 +1941,53 @@
       <c r="AK8" s="9"/>
     </row>
     <row r="9" spans="1:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
-      <c r="Y9" s="40"/>
-      <c r="Z9" s="40"/>
-      <c r="AA9" s="40"/>
-      <c r="AB9" s="40"/>
-      <c r="AC9" s="40"/>
-      <c r="AD9" s="40"/>
-      <c r="AE9" s="40"/>
-      <c r="AF9" s="40"/>
-      <c r="AG9" s="40"/>
-      <c r="AH9" s="40"/>
-      <c r="AI9" s="40"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>77</v>
@@ -2007,57 +2032,57 @@
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="35">
-        <v>0</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="38"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="33"/>
+      <c r="AF11" s="33"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="33"/>
+      <c r="AI11" s="33"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>11</v>
@@ -2102,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>12</v>
@@ -2147,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D14" s="29">
         <v>0</v>
@@ -2181,11 +2206,11 @@
       <c r="AE14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AF14" s="33">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="33"/>
-      <c r="AH14" s="33"/>
+      <c r="AF14" s="34">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="34"/>
+      <c r="AH14" s="34"/>
       <c r="AI14" s="15" t="s">
         <v>13</v>
       </c>
@@ -2198,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>15</v>
@@ -2243,20 +2268,20 @@
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="33">
-        <v>0</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="34"/>
+        <v>95</v>
+      </c>
+      <c r="D16" s="34">
+        <v>0</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
       <c r="L16" s="22" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
@@ -2290,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>33</v>
@@ -2335,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>34</v>
@@ -2380,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>35</v>
@@ -2425,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>36</v>
@@ -2470,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>37</v>
@@ -2507,8 +2532,71 @@
       <c r="AH21" s="22"/>
       <c r="AI21" s="22"/>
     </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="22"/>
+      <c r="X22" s="22"/>
+      <c r="Y22" s="22"/>
+      <c r="Z22" s="22"/>
+      <c r="AA22" s="22"/>
+      <c r="AB22" s="22"/>
+      <c r="AC22" s="22"/>
+      <c r="AD22" s="22"/>
+      <c r="AE22" s="22"/>
+      <c r="AF22" s="22"/>
+      <c r="AG22" s="22"/>
+      <c r="AH22" s="22"/>
+      <c r="AI22" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="D15:AI15"/>
+    <mergeCell ref="L16:AI16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D14:AD14"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="L11:AI11"/>
+    <mergeCell ref="D12:AI12"/>
+    <mergeCell ref="D13:AI13"/>
+    <mergeCell ref="AF14:AH14"/>
+    <mergeCell ref="L2:AI2"/>
+    <mergeCell ref="J3:S3"/>
+    <mergeCell ref="X3:AI3"/>
+    <mergeCell ref="D4:S4"/>
+    <mergeCell ref="T4:AI4"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="D22:AI22"/>
     <mergeCell ref="D10:S10"/>
     <mergeCell ref="T10:AI10"/>
     <mergeCell ref="R7:AI7"/>
@@ -2519,28 +2607,11 @@
     <mergeCell ref="D8:S8"/>
     <mergeCell ref="A6:AI6"/>
     <mergeCell ref="A9:AI9"/>
-    <mergeCell ref="L2:AI2"/>
-    <mergeCell ref="J3:S3"/>
-    <mergeCell ref="X3:AI3"/>
-    <mergeCell ref="D4:S4"/>
-    <mergeCell ref="T4:AI4"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="D3:I3"/>
     <mergeCell ref="D17:AI17"/>
     <mergeCell ref="D18:AI18"/>
     <mergeCell ref="D19:AI19"/>
     <mergeCell ref="D20:AI20"/>
     <mergeCell ref="D21:AI21"/>
-    <mergeCell ref="D15:AI15"/>
-    <mergeCell ref="L16:AI16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="D14:AD14"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="L11:AI11"/>
-    <mergeCell ref="D12:AI12"/>
-    <mergeCell ref="D13:AI13"/>
-    <mergeCell ref="AF14:AH14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2550,10 +2621,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA410207-3AA3-4D83-9908-FDFA42DD0A6C}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2571,10 +2642,10 @@
         <v>76</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>44</v>
@@ -2681,14 +2752,14 @@
         <v>0</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="45">
-        <v>0</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+        <v>92</v>
+      </c>
+      <c r="D2" s="44">
+        <v>0</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="7">
         <v>0</v>
       </c>
@@ -2705,12 +2776,12 @@
         <v>0</v>
       </c>
       <c r="M2" s="46" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="N2" s="46"/>
       <c r="O2" s="46"/>
       <c r="P2" s="46" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="Q2" s="46"/>
       <c r="R2" s="46"/>
@@ -2726,69 +2797,91 @@
       <c r="AB2" s="47">
         <v>0</v>
       </c>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
     </row>
     <row r="3" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
-    </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="44">
+        <v>0</v>
+      </c>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19">
+        <v>1</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="47">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="44"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
+    </row>
+    <row r="4" spans="1:35" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B4" s="18">
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="45">
-        <v>0</v>
-      </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+        <v>92</v>
+      </c>
+      <c r="D4" s="44">
+        <v>0</v>
+      </c>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="7">
         <v>0</v>
       </c>
@@ -2805,12 +2898,12 @@
         <v>0</v>
       </c>
       <c r="M4" s="46" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="N4" s="46"/>
       <c r="O4" s="46"/>
       <c r="P4" s="46" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="Q4" s="46"/>
       <c r="R4" s="46"/>
@@ -2826,30 +2919,30 @@
       <c r="AB4" s="47">
         <v>0</v>
       </c>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="45"/>
-      <c r="AF4" s="45"/>
-      <c r="AG4" s="45"/>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="45"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="45">
-        <v>0</v>
-      </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="44"/>
+      <c r="AH4" s="44"/>
+      <c r="AI4" s="44"/>
+    </row>
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0</v>
+      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="7">
         <v>0</v>
       </c>
@@ -2865,17 +2958,13 @@
       <c r="L5" s="9">
         <v>0</v>
       </c>
-      <c r="M5" s="7">
-        <v>1</v>
-      </c>
-      <c r="N5" s="7">
-        <v>1</v>
-      </c>
-      <c r="O5" s="7">
-        <v>1</v>
-      </c>
+      <c r="M5" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
       <c r="P5" s="46" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="46"/>
       <c r="R5" s="46"/>
@@ -2888,99 +2977,93 @@
       <c r="Y5" s="46"/>
       <c r="Z5" s="46"/>
       <c r="AA5" s="46"/>
+      <c r="AB5" s="47">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="44"/>
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="44"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="42">
-        <v>0</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+        <v>97</v>
+      </c>
+      <c r="D6" s="44">
+        <v>0</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="19">
         <v>1</v>
       </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
-        <v>0</v>
-      </c>
-      <c r="L6" s="44">
-        <v>0</v>
-      </c>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="7">
+      <c r="K6" s="19">
         <v>1</v>
       </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1</v>
+      </c>
+      <c r="P6" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="46"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+        <v>97</v>
+      </c>
+      <c r="D7" s="39">
+        <v>0</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="7">
         <v>0</v>
@@ -2988,128 +3071,206 @@
       <c r="K7" s="7">
         <v>0</v>
       </c>
-      <c r="L7" s="7">
-        <v>1</v>
-      </c>
-      <c r="M7" s="7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="7">
-        <v>1</v>
-      </c>
-      <c r="O7" s="7">
-        <v>1</v>
-      </c>
-      <c r="P7" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="43"/>
+      <c r="L7" s="45">
+        <v>0</v>
+      </c>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="39"/>
+      <c r="Z7" s="39"/>
+      <c r="AA7" s="40"/>
       <c r="AB7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="42">
-        <v>0</v>
-      </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
-      <c r="AA8" s="42"/>
-      <c r="AB8" s="42"/>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="43"/>
-      <c r="AF8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="39">
+        <v>0</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>1</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1</v>
+      </c>
+      <c r="P8" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="39"/>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="40"/>
+      <c r="AB8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="39">
+        <v>0</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="39"/>
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="39"/>
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="39"/>
+      <c r="AD9" s="39"/>
+      <c r="AE9" s="40"/>
+      <c r="AF9" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AG8" s="7" t="s">
+      <c r="AG9" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AH8" s="7" t="s">
+      <c r="AH9" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AI8" s="7" t="s">
+      <c r="AI9" s="7" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A3:AI3"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="P7:AA7"/>
-    <mergeCell ref="D8:AE8"/>
+  <mergeCells count="23">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:AA3"/>
+    <mergeCell ref="AB3:AI3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:AA4"/>
+    <mergeCell ref="AB4:AI4"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="P8:AA8"/>
+    <mergeCell ref="D9:AE9"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:AA2"/>
     <mergeCell ref="AB2:AI2"/>
-    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="P6:AA6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="L7:AA7"/>
+    <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:AA5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="L6:AA6"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:AA4"/>
-    <mergeCell ref="AB4:AI4"/>
+    <mergeCell ref="AB5:AI5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3121,7 +3282,7 @@
   <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,10 +3300,10 @@
         <v>76</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>44</v>
@@ -3247,10 +3408,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>16</v>
@@ -3295,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D3" s="49">
         <v>0</v>
@@ -3342,7 +3503,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D4" s="51">
         <v>0</v>
@@ -3386,10 +3547,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D5" s="51">
         <v>0</v>
@@ -3436,41 +3597,41 @@
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="40">
-        <v>0</v>
-      </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="40"/>
-      <c r="Z6" s="40"/>
-      <c r="AA6" s="40"/>
-      <c r="AB6" s="40"/>
-      <c r="AC6" s="40"/>
-      <c r="AD6" s="40"/>
-      <c r="AE6" s="40"/>
-      <c r="AF6" s="40"/>
-      <c r="AG6" s="40"/>
-      <c r="AH6" s="41"/>
+        <v>95</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="42"/>
       <c r="AI6" s="7" t="s">
         <v>20</v>
       </c>
@@ -3483,41 +3644,41 @@
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="40"/>
-      <c r="Z7" s="40"/>
-      <c r="AA7" s="40"/>
-      <c r="AB7" s="40"/>
-      <c r="AC7" s="40"/>
-      <c r="AD7" s="40"/>
-      <c r="AE7" s="40"/>
-      <c r="AF7" s="40"/>
-      <c r="AG7" s="40"/>
-      <c r="AH7" s="41"/>
+        <v>92</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="38"/>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="38"/>
+      <c r="AF7" s="38"/>
+      <c r="AG7" s="38"/>
+      <c r="AH7" s="42"/>
       <c r="AI7" s="7" t="s">
         <v>21</v>
       </c>

</xml_diff>